<commit_message>
Fix scrapers: add missing imports, reference extraction methods, and BeautifulSoup compatibility
</commit_message>
<xml_diff>
--- a/output/test_tracker.xlsx
+++ b/output/test_tracker.xlsx
@@ -685,7 +685,7 @@
       </c>
       <c r="P2" s="3" t="inlineStr">
         <is>
-          <t>2025-08-14 01:52</t>
+          <t>2025-08-14 03:48</t>
         </is>
       </c>
       <c r="Q2" s="3" t="inlineStr">
@@ -778,7 +778,7 @@
       </c>
       <c r="P3" s="3" t="inlineStr">
         <is>
-          <t>2025-08-14 01:52</t>
+          <t>2025-08-14 03:48</t>
         </is>
       </c>
       <c r="Q3" s="3" t="inlineStr">
@@ -871,7 +871,7 @@
       </c>
       <c r="P4" s="4" t="inlineStr">
         <is>
-          <t>2025-08-14 01:52</t>
+          <t>2025-08-14 03:48</t>
         </is>
       </c>
       <c r="Q4" s="4" t="inlineStr">
@@ -964,7 +964,7 @@
       </c>
       <c r="P5" s="4" t="inlineStr">
         <is>
-          <t>2025-08-14 01:52</t>
+          <t>2025-08-14 03:48</t>
         </is>
       </c>
       <c r="Q5" s="4" t="inlineStr">
@@ -1053,7 +1053,7 @@
       </c>
       <c r="P6" s="5" t="inlineStr">
         <is>
-          <t>2025-08-14 01:52</t>
+          <t>2025-08-14 03:48</t>
         </is>
       </c>
       <c r="Q6" s="5" t="inlineStr">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="B4" s="6" t="inlineStr">
         <is>
-          <t>2025-08-14 01:52:30</t>
+          <t>2025-08-14 03:48:11</t>
         </is>
       </c>
     </row>

</xml_diff>